<commit_message>
Lagt in tider jag kan
</commit_message>
<xml_diff>
--- a/inte_schema.xlsx
+++ b/inte_schema.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macha\OneDrive\Dokument\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewett\inte\inte-kommando\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="12">
   <si>
     <t>Schema</t>
   </si>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -171,11 +171,11 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,13 +493,13 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:11" ht="26" x14ac:dyDescent="0.6">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -514,56 +514,56 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B6" s="2">
+      <c r="B6" s="5">
         <v>42660</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2">
+      <c r="C6" s="6"/>
+      <c r="D6" s="5">
         <v>42661</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2">
+      <c r="E6" s="6"/>
+      <c r="F6" s="5">
         <v>42662</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="2">
+      <c r="G6" s="6"/>
+      <c r="H6" s="5">
         <v>42663</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="2">
+      <c r="I6" s="6"/>
+      <c r="J6" s="5">
         <v>42664</v>
       </c>
-      <c r="K6" s="3"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="5" t="s">
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -647,68 +647,88 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B14" s="2">
+      <c r="B14" s="5">
         <v>42667</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2">
+      <c r="C14" s="6"/>
+      <c r="D14" s="5">
         <v>42668</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="2">
+      <c r="E14" s="6"/>
+      <c r="F14" s="5">
         <v>42669</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="2">
+      <c r="G14" s="6"/>
+      <c r="H14" s="5">
         <v>42670</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="2">
+      <c r="I14" s="6"/>
+      <c r="J14" s="5">
         <v>42671</v>
       </c>
-      <c r="K14" s="3"/>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K15" s="5" t="s">
+      <c r="B15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -794,29 +814,49 @@
       <c r="A20" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Lagt in de tider jag kan
</commit_message>
<xml_diff>
--- a/inte_schema.xlsx
+++ b/inte_schema.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewett\inte\inte-kommando\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4095"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="13">
   <si>
     <t>Schema</t>
   </si>
@@ -60,13 +55,16 @@
   </si>
   <si>
     <t>:D</t>
+  </si>
+  <si>
+    <t>:D - :(</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,7 +234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -288,7 +286,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -482,38 +480,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="26" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:11" ht="26.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11">
       <c r="B6" s="5">
         <v>42660</v>
       </c>
@@ -535,7 +533,7 @@
       </c>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -567,7 +565,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -598,22 +596,42 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -628,7 +646,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -643,7 +661,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -678,7 +696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11">
       <c r="B14" s="5">
         <v>42667</v>
       </c>
@@ -700,7 +718,7 @@
       </c>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11">
       <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
@@ -732,7 +750,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -765,22 +783,42 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -795,7 +833,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -810,7 +848,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>5</v>
       </c>

</xml_diff>